<commit_message>
more progress on paper figs, inc analytical soln
</commit_message>
<xml_diff>
--- a/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
+++ b/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/High-Plains/modeling headway FA22/manuscript figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16C13CC5-6998-9B48-A19F-C7667C7A4BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D92CFD-1078-F54A-A70E-91C0156A8F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="600" windowWidth="28000" windowHeight="16640" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
+    <workbookView xWindow="380" yWindow="580" windowWidth="28000" windowHeight="15960" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -439,11 +439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA74029-AED1-9545-9068-39E1E9E1F4C4}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,13 +544,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="F3" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G3">
-        <v>1E-4</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="H3">
         <f>B3 * C3</f>
@@ -576,13 +576,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>1E-8</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
       <c r="G4">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="H4">
         <f>B4 * C4</f>
@@ -601,8 +601,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
       <c r="D5">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1E-8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G5">
+        <v>1E-4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H10" si="1">B5 * C5</f>
+        <v>16666666666.666664</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I10" si="2" xml:space="preserve"> H5/(SQRT(2.65 * 9.81 * (D5^5)))</f>
+        <v>118621431666566.12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -613,8 +633,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
       <c r="D6">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G6">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>16666666666.666664</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>118621431666566.12</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -625,8 +665,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
       <c r="D7">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G7">
+        <v>1E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>16666666666.666664</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>118621431666566.12</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -637,8 +697,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
       <c r="D8">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1E-8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G8">
+        <v>1E-4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>33333333333.333328</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>237242863333132.25</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -649,8 +729,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
       <c r="D9">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G9">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>33333333333.333328</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>237242863333132.25</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -661,128 +761,28 @@
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
       <c r="D10">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>100000</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D11">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>100000</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>100000</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D13">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>100000</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D14">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>100000</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>100000</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D16">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>100000</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D17">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>100000</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D18">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>100000</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D19">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>100000</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="D20">
-        <v>1.4999999999999999E-2</v>
+      <c r="E10" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G10">
+        <v>1E-3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>33333333333.333328</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>237242863333132.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
figured out analytical solution
</commit_message>
<xml_diff>
--- a/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
+++ b/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/High-Plains/modeling headway FA22/manuscript figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D92CFD-1078-F54A-A70E-91C0156A8F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2584F245-1A78-8D4C-B0F2-6DC9F3BB38DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="580" windowWidth="28000" windowHeight="15960" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
+    <workbookView xWindow="340" yWindow="640" windowWidth="32520" windowHeight="17820" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Area</t>
   </si>
@@ -78,13 +78,16 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Q per s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,13 +103,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,10 +143,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,21 +468,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA74029-AED1-9545-9068-39E1E9E1F4C4}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -479,25 +508,28 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100000</v>
       </c>
@@ -521,79 +553,125 @@
         <v>1E-4</v>
       </c>
       <c r="H2">
-        <f>B2 * C2</f>
+        <f>A2 * B2</f>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I2">
+        <f>H2/(31500000)</f>
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J2">
+        <f xml:space="preserve"> I2/(SQRT(2.65 * 9.81 * (D2^5)))</f>
+        <v>75315194708.930893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>100000</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B11" si="0" xml:space="preserve"> (1/3) * (A3^(2))</f>
         <v>3333333333.333333</v>
       </c>
-      <c r="I2">
-        <f xml:space="preserve"> H2/(SQRT(2.65 * 9.81 * (D2^5)))</f>
-        <v>23724286333313.227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="H3" s="6">
+        <f>A3 * B3</f>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="1">H3/(31500000)</f>
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J3" s="6">
+        <f xml:space="preserve"> I3/(SQRT(2.65 * 9.81 * (D3^5)))</f>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1.186099E-2</v>
+      </c>
+      <c r="L3" s="5">
+        <v>836.04862337999998</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.12394831000000001</v>
+      </c>
+      <c r="N3">
+        <f>L3/D3</f>
+        <v>55736.574892000004</v>
+      </c>
+      <c r="O3">
+        <f>M3/D3</f>
+        <v>8.2632206666666672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>100000</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B20" si="0" xml:space="preserve"> (1/3) * (A3^(2))</f>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="G3">
-        <v>5.5000000000000003E-4</v>
-      </c>
-      <c r="H3">
-        <f>B3 * C3</f>
-        <v>3333333333.333333</v>
-      </c>
-      <c r="I3">
-        <f xml:space="preserve"> H3/(SQRT(2.65 * 9.81 * (D3^5)))</f>
-        <v>23724286333313.227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>100000</v>
-      </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="7">
         <v>1E-4</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>1E-3</v>
       </c>
-      <c r="H4">
-        <f>B4 * C4</f>
-        <v>3333333333.333333</v>
+      <c r="H4" s="6">
+        <f>A4 * B4</f>
+        <v>333333333333333.31</v>
       </c>
       <c r="I4">
-        <f xml:space="preserve"> H4/(SQRT(2.65 * 9.81 * (D4^5)))</f>
-        <v>23724286333313.227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J4" s="6">
+        <f xml:space="preserve"> I4/(SQRT(2.65 * 9.81 * (D4^5)))</f>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K4" s="5">
+        <v>4.4802599999999998E-3</v>
+      </c>
+      <c r="L4" s="5">
+        <v>268.49954416000003</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.32813978999999999</v>
+      </c>
+      <c r="N4">
+        <f>L4/D4</f>
+        <v>17899.969610666671</v>
+      </c>
+      <c r="O4">
+        <f>M4/D4</f>
+        <v>21.875986000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>100000</v>
       </c>
@@ -617,79 +695,125 @@
         <v>1E-4</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H10" si="1">B5 * C5</f>
-        <v>16666666666.666664</v>
+        <f t="shared" ref="H5:I12" si="2">A5 * B5</f>
+        <v>333333333333333.31</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I10" si="2" xml:space="preserve"> H5/(SQRT(2.65 * 9.81 * (D5^5)))</f>
-        <v>118621431666566.12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J12" si="3" xml:space="preserve"> I5/(SQRT(2.65 * 9.81 * (D5^5)))</f>
+        <v>75315194708.930893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>100000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="7">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>5.5000000000000003E-4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
+        <f t="shared" si="2"/>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
-        <v>16666666666.666664</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>118621431666566.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="3"/>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K6" s="5">
+        <v>2.97679E-3</v>
+      </c>
+      <c r="L6" s="6">
+        <v>833.23451827999997</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.49387025000000001</v>
+      </c>
+      <c r="N6">
+        <f>L6/D6</f>
+        <v>55548.967885333332</v>
+      </c>
+      <c r="O6">
+        <f>M6/D6</f>
+        <v>32.924683333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>100000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="7">
         <v>1E-4</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>1E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
+        <f t="shared" si="2"/>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I7" s="6">
         <f t="shared" si="1"/>
-        <v>16666666666.666664</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>118621431666566.12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="3"/>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.1276000000000001E-3</v>
+      </c>
+      <c r="L7" s="5">
+        <v>268.47744347999998</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1.30378711</v>
+      </c>
+      <c r="N7">
+        <f>L7/D7</f>
+        <v>17898.496231999998</v>
+      </c>
+      <c r="O7">
+        <f>M7/D7</f>
+        <v>86.919140666666678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100000</v>
       </c>
@@ -713,76 +837,194 @@
         <v>1E-4</v>
       </c>
       <c r="H8">
+        <f t="shared" si="2"/>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
-        <v>33333333333.333328</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>237242863333132.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9">
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>75315194708.930893</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>100000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="7">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>5.5000000000000003E-4</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
+        <f t="shared" si="2"/>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I9" s="6">
         <f t="shared" si="1"/>
-        <v>33333333333.333328</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>237242863333132.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10">
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="3"/>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1.6416200000000001E-3</v>
+      </c>
+      <c r="L9" s="5">
+        <v>832.22515911000005</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0.89554990000000001</v>
+      </c>
+      <c r="N9">
+        <f>L9/D9</f>
+        <v>55481.677274000009</v>
+      </c>
+      <c r="O9">
+        <f>M9/D9</f>
+        <v>59.703326666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>100000</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>3333333333.333333</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="7">
         <v>1E-4</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>1E-3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="6">
+        <f t="shared" si="2"/>
+        <v>333333333333333.31</v>
+      </c>
+      <c r="I10" s="6">
         <f t="shared" si="1"/>
-        <v>33333333333.333328</v>
-      </c>
-      <c r="I10">
+        <v>10582010.582010582</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="3"/>
+        <v>75315194708.930893</v>
+      </c>
+      <c r="K10" s="5">
+        <v>6.2246999999999997E-4</v>
+      </c>
+      <c r="L10" s="5">
+        <v>268.47027680999997</v>
+      </c>
+      <c r="M10" s="5">
+        <v>2.36179571</v>
+      </c>
+      <c r="N10">
+        <f>L10/D10</f>
+        <v>17898.018453999997</v>
+      </c>
+      <c r="O10">
+        <f>M10/D10</f>
+        <v>157.45304733333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="3">
+        <f xml:space="preserve"> (1/3) * (A11^(1.5))</f>
+        <v>10540925.533894591</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="2"/>
-        <v>237242863333132.25</v>
+        <v>1054092553389.4591</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>33463.255663157433</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="3"/>
+        <v>238167557.69928372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>100000</v>
+      </c>
+      <c r="B12" s="8">
+        <f xml:space="preserve"> (1/3) * (A12^(1.5))</f>
+        <v>10540925.533894591</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G12" s="8">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="2"/>
+        <v>1054092553389.4591</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="1"/>
+        <v>33463.255663157433</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="3"/>
+        <v>238167557.69928372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lateral supply with instant hillslopes, and new experiments for paper
</commit_message>
<xml_diff>
--- a/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
+++ b/modeling headway FA22/manuscript figs/alluvial_geom_experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/High-Plains/modeling headway FA22/manuscript figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F44544-171E-7A4A-B434-3960CEED1BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45640DFA-640F-5641-B932-1F30D69CD4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="35440" windowHeight="19020" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="36040" windowHeight="18360" xr2:uid="{A46A4A44-CAAD-2B4F-AD16-E348C8322479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +529,7 @@
         <v>50000</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:B11" si="0" xml:space="preserve"> (1/3) * (A2^(2))</f>
+        <f xml:space="preserve"> (1/3) * (A2^(2))</f>
         <v>833333333.33333325</v>
       </c>
       <c r="C2" s="2">
@@ -552,11 +552,11 @@
         <v>833333333.33333325</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I13" si="1">H2/(31500000)</f>
+        <f>H2/(31500000)</f>
         <v>26.455026455026452</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" ref="J2:J16" si="2" xml:space="preserve"> I2/(SQRT(2.65 * 9.81 * (D2^5)))</f>
+        <f xml:space="preserve"> I2/(SQRT(2.65 * 9.81 * (D2^5)))</f>
         <v>518860.67882412398</v>
       </c>
       <c r="K2" s="4">
@@ -575,11 +575,11 @@
         <v>1.693534156770243E-2</v>
       </c>
       <c r="O2" s="2">
-        <f>M2/D2</f>
+        <f t="shared" ref="O2:O31" si="0">M2/D2</f>
         <v>460352.34212778124</v>
       </c>
       <c r="P2" s="2">
-        <f>N2/D2</f>
+        <f t="shared" ref="P2:P31" si="1">N2/D2</f>
         <v>1.6935341567702429</v>
       </c>
     </row>
@@ -588,7 +588,7 @@
         <v>50000</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B2:B11" si="2" xml:space="preserve"> (1/3) * (A3^(2))</f>
         <v>833333333.33333325</v>
       </c>
       <c r="C3" s="2">
@@ -611,34 +611,34 @@
         <v>833333333.33333325</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I2:I13" si="4">H3/(31500000)</f>
         <v>26.455026455026452</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J2:J16" si="5" xml:space="preserve"> I3/(SQRT(2.65 * 9.81 * (D3^5)))</f>
         <v>518860.67882412398</v>
       </c>
       <c r="K3" s="4">
         <v>9.8458437154767993E-3</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L31" si="4">0.15 * K3^(0.25)</f>
+        <f t="shared" ref="L3:L31" si="6">0.15 * K3^(0.25)</f>
         <v>4.7250291651040915E-2</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" ref="M3:M31" si="5">(2.61* I3 * K3^(7/6))/(D3 ^ (3/2))</f>
+        <f>(2.61* I3 * K3^(7/6))/(D3 ^ (3/2))</f>
         <v>314.7341017403092</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N31" si="6">(1.98 * L3 * D3) / K3</f>
+        <f>(1.98 * L3 * D3) / K3</f>
         <v>9.502037628527446E-2</v>
       </c>
       <c r="O3" s="2">
-        <f>M3/D3</f>
+        <f t="shared" si="0"/>
         <v>31473.41017403092</v>
       </c>
       <c r="P3" s="2">
-        <f>N3/D3</f>
+        <f t="shared" si="1"/>
         <v>9.5020376285274466</v>
       </c>
     </row>
@@ -647,7 +647,7 @@
         <v>50000</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C4" s="2">
@@ -670,34 +670,34 @@
         <v>833333333.33333325</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>26.455026455026452</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>518860.67882412398</v>
       </c>
       <c r="K4" s="4">
         <v>3.3216993839247103E-2</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.403705346702844E-2</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="M3:M31" si="7">(2.61* I4 * K4^(7/6))/(D4 ^ (3/2))</f>
         <v>1300.3764260727032</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="N3:N31" si="8">(1.98 * L4 * D4) / K4</f>
         <v>3.8171234422455562E-2</v>
       </c>
       <c r="O4" s="2">
-        <f>M4/D4</f>
+        <f t="shared" si="0"/>
         <v>130037.64260727032</v>
       </c>
       <c r="P4" s="2">
-        <f>N4/D4</f>
+        <f t="shared" si="1"/>
         <v>3.8171234422455562</v>
       </c>
     </row>
@@ -706,7 +706,7 @@
         <v>50000</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C5" s="2">
@@ -729,34 +729,34 @@
         <v>4166666666.666666</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>132.27513227513225</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2594303.3941206196</v>
       </c>
       <c r="K5" s="4">
         <v>2.4781967968447098E-3</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3467649101036952E-2</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>314.73410174364511</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.26739581499106246</v>
       </c>
       <c r="O5" s="2">
-        <f>M5/D5</f>
+        <f t="shared" si="0"/>
         <v>31473.410174364511</v>
       </c>
       <c r="P5" s="2">
-        <f>N5/D5</f>
+        <f t="shared" si="1"/>
         <v>26.739581499106247</v>
       </c>
     </row>
@@ -765,7 +765,7 @@
         <v>50000</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C6" s="2">
@@ -788,34 +788,34 @@
         <v>4166666666.666666</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>132.27513227513225</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2594303.3941206196</v>
       </c>
       <c r="K6" s="4">
         <v>1.6369783037807699E-3</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.0171853470732299E-2</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194.01506597743091</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.36494234367110212</v>
       </c>
       <c r="O6" s="2">
-        <f>M6/D6</f>
+        <f t="shared" si="0"/>
         <v>19401.50659774309</v>
       </c>
       <c r="P6" s="2">
-        <f>N6/D6</f>
+        <f t="shared" si="1"/>
         <v>36.494234367110209</v>
       </c>
     </row>
@@ -824,7 +824,7 @@
         <v>50000</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C7" s="2">
@@ -847,34 +847,34 @@
         <v>4166666666.666666</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>132.27513227513225</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2594303.3941206196</v>
       </c>
       <c r="K7" s="4">
         <v>2.4707729540707001E-2</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.9470209544088805E-2</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4603.5234213273125</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.7657561858646787E-2</v>
       </c>
       <c r="O7" s="2">
-        <f>M7/D7</f>
+        <f t="shared" si="0"/>
         <v>460352.34213273122</v>
       </c>
       <c r="P7" s="2">
-        <f>N7/D7</f>
+        <f t="shared" si="1"/>
         <v>4.7657561858646789</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
         <v>50000</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C8" s="2">
@@ -906,34 +906,34 @@
         <v>4166666666.666666</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>132.27513227513225</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2594303.3941206196</v>
       </c>
       <c r="K8" s="4">
         <v>8.3607103780377594E-3</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.5357807539522947E-2</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1300.3764260734392</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.10741725866281389</v>
       </c>
       <c r="O8" s="2">
-        <f>M8/D8</f>
+        <f t="shared" si="0"/>
         <v>130037.64260734392</v>
       </c>
       <c r="P8" s="2">
-        <f>N8/D8</f>
+        <f t="shared" si="1"/>
         <v>10.741725866281389</v>
       </c>
     </row>
@@ -942,7 +942,7 @@
         <v>40000</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>533333333.33333331</v>
       </c>
       <c r="C9" s="2">
@@ -965,34 +965,34 @@
         <v>5333333333.333333</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>169.31216931216929</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3320708.3444743934</v>
       </c>
       <c r="K9" s="4">
         <v>5.4844001502497098E-3</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.0820050961478005E-2</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1017.7614677889519</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.14737017484044537</v>
       </c>
       <c r="O9" s="2">
-        <f>M9/D9</f>
+        <f t="shared" si="0"/>
         <v>101776.14677889518</v>
       </c>
       <c r="P9" s="2">
-        <f>N9/D9</f>
+        <f t="shared" si="1"/>
         <v>14.737017484044538</v>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
         <v>25000</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>208333333.33333331</v>
       </c>
       <c r="C10" s="2">
@@ -1024,34 +1024,34 @@
         <v>2083333333.333333</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>66.137566137566125</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1297151.6970603098</v>
       </c>
       <c r="K10" s="4">
         <v>7.6199231402715598E-3</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.4317872809782541E-2</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>583.48684898541785</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.11515783892833623</v>
       </c>
       <c r="O10" s="2">
-        <f>M10/D10</f>
+        <f t="shared" si="0"/>
         <v>58348.684898541782</v>
       </c>
       <c r="P10" s="2">
-        <f>N10/D10</f>
+        <f t="shared" si="1"/>
         <v>11.515783892833623</v>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
         <v>25000</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>208333333.33333331</v>
       </c>
       <c r="C11" s="2">
@@ -1083,34 +1083,34 @@
         <v>2083333333.333333</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>66.137566137566125</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>83212.320164172197</v>
       </c>
       <c r="K11" s="4">
         <v>7.6199231402715598E-3</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.4317872809782541E-2</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>112.29209644344584</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.34547351678500865</v>
       </c>
       <c r="O11" s="2">
-        <f>M11/D11</f>
+        <f t="shared" si="0"/>
         <v>3743.0698814481948</v>
       </c>
       <c r="P11" s="2">
-        <f>N11/D11</f>
+        <f t="shared" si="1"/>
         <v>11.515783892833623</v>
       </c>
     </row>
@@ -1142,34 +1142,34 @@
         <v>8333333333.3333321</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>264.5502645502645</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5188606.7882412393</v>
       </c>
       <c r="K12" s="4">
         <v>3.3216993839188899E-2</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.4037053467000393E-2</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13003.764260700453</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.8171234422505723E-2</v>
       </c>
       <c r="O12" s="2">
-        <f>M12/D12</f>
+        <f t="shared" si="0"/>
         <v>1300376.4260700452</v>
       </c>
       <c r="P12" s="2">
-        <f>N12/D12</f>
+        <f t="shared" si="1"/>
         <v>3.8171234422505722</v>
       </c>
     </row>
@@ -1201,34 +1201,34 @@
         <v>8333333333.3333321</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>264.5502645502645</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5188606.7882412393</v>
       </c>
       <c r="K13" s="4">
         <v>1.3639772545589899E-2</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.1261704300207843E-2</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4603.523421050998</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.4413392287269911E-2</v>
       </c>
       <c r="O13" s="2">
-        <f>M13/D13</f>
+        <f t="shared" si="0"/>
         <v>460352.34210509981</v>
       </c>
       <c r="P13" s="2">
-        <f>N13/D13</f>
+        <f t="shared" si="1"/>
         <v>7.4413392287269913</v>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
         <v>50000</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" ref="B14" si="7" xml:space="preserve"> (1/3) * (A14^(2))</f>
+        <f t="shared" ref="B14" si="9" xml:space="preserve"> (1/3) * (A14^(2))</f>
         <v>833333333.33333325</v>
       </c>
       <c r="C14" s="2">
@@ -1260,34 +1260,34 @@
         <v>8333333333.3333321</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" ref="I14" si="8">H14/(31500000)</f>
+        <f t="shared" ref="I14" si="10">H14/(31500000)</f>
         <v>264.5502645502645</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>917224.76121898333</v>
       </c>
       <c r="K14" s="4">
         <v>1.3639772545589899E-2</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.1261704300207843E-2</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1627.5913141881272</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.14882678457453982</v>
       </c>
       <c r="O14" s="2">
-        <f>M14/D14</f>
+        <f t="shared" si="0"/>
         <v>81379.56570940635</v>
       </c>
       <c r="P14" s="2">
-        <f>N14/D14</f>
+        <f t="shared" si="1"/>
         <v>7.4413392287269913</v>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
         <v>50000</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15:B31" si="9" xml:space="preserve"> (1/3) * (A15^(2))</f>
+        <f t="shared" ref="B15:B31" si="11" xml:space="preserve"> (1/3) * (A15^(2))</f>
         <v>833333333.33333325</v>
       </c>
       <c r="C15" s="2">
@@ -1319,34 +1319,34 @@
         <v>12499999999.999998</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" ref="I15:I31" si="10">H15/(31500000)</f>
+        <f t="shared" ref="I15:I31" si="12">H15/(31500000)</f>
         <v>396.82539682539675</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1375837.1418284748</v>
       </c>
       <c r="K15" s="4">
         <v>9.6354447013218304E-3</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.6995816553405068E-2</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1627.5913143504797</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.19314462312876293</v>
       </c>
       <c r="O15" s="2">
-        <f>M15/D15</f>
+        <f t="shared" si="0"/>
         <v>81379.56571752399</v>
       </c>
       <c r="P15" s="2">
-        <f>N15/D15</f>
+        <f t="shared" si="1"/>
         <v>9.6572311564381472</v>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
         <v>50000</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C16" s="2">
@@ -1378,34 +1378,34 @@
         <v>12499999999.999998</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>396.82539682539675</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>44026788.538511194</v>
       </c>
       <c r="K16" s="4">
         <v>9.6354447014564294E-3</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.6995816553569193E-2</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>13020.730515016032</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.8286155781684846E-2</v>
       </c>
       <c r="O16" s="2">
-        <f>M16/D16</f>
+        <f t="shared" si="0"/>
         <v>2604146.1030032062</v>
       </c>
       <c r="P16" s="2">
-        <f>N16/D16</f>
+        <f t="shared" si="1"/>
         <v>9.6572311563369695</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
         <v>40000</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>533333333.33333331</v>
       </c>
       <c r="C17" s="2">
@@ -1437,34 +1437,34 @@
         <v>5333333333.333333</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>169.31216931216929</v>
       </c>
       <c r="J17" s="2">
-        <f xml:space="preserve"> I17/(SQRT(2.65 * 9.81 * (D17^5)))</f>
+        <f t="shared" ref="J17:J31" si="13" xml:space="preserve"> I17/(SQRT(2.65 * 9.81 * (D17^5)))</f>
         <v>3320708.3444743934</v>
       </c>
       <c r="K17" s="4">
         <v>1.6317451808219599E-2</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.361105377103393E-2</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3631.530895771718</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.5052979910243239E-2</v>
       </c>
       <c r="O17" s="2">
-        <f>M17/D17</f>
+        <f t="shared" si="0"/>
         <v>363153.08957717178</v>
       </c>
       <c r="P17" s="2">
-        <f>N17/D17</f>
+        <f t="shared" si="1"/>
         <v>6.5052979910243236</v>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
         <v>40000</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>533333333.33333331</v>
       </c>
       <c r="C18" s="2">
@@ -1496,34 +1496,34 @@
         <v>5333333333.333333</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>169.31216931216929</v>
       </c>
       <c r="J18" s="2">
-        <f xml:space="preserve"> I18/(SQRT(2.65 * 9.81 * (D18^5)))</f>
+        <f t="shared" si="13"/>
         <v>1205043.1153428941</v>
       </c>
       <c r="K18" s="4">
         <v>1.6317451808219599E-2</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.361105377103393E-2</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1976.7550399540087</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.7579469865364865E-2</v>
       </c>
       <c r="O18" s="2">
-        <f>M18/D18</f>
+        <f t="shared" si="0"/>
         <v>131783.66933026726</v>
       </c>
       <c r="P18" s="2">
-        <f>N18/D18</f>
+        <f t="shared" si="1"/>
         <v>6.5052979910243245</v>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
         <v>50000</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C19" s="2">
@@ -1555,34 +1555,34 @@
         <v>8333333333.3333321</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>264.5502645502645</v>
       </c>
       <c r="J19" s="2">
-        <f xml:space="preserve"> I19/(SQRT(2.65 * 9.81 * (D19^5)))</f>
+        <f t="shared" si="13"/>
         <v>5188606.7882412393</v>
       </c>
       <c r="K19" s="4">
         <v>1.36807554819461E-3</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8848203916580557E-2</v>
       </c>
       <c r="M19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>314.73410176685422</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.41751673604727135</v>
       </c>
       <c r="O19" s="2">
-        <f>M19/D19</f>
+        <f t="shared" si="0"/>
         <v>31473.410176685422</v>
       </c>
       <c r="P19" s="2">
-        <f>N19/D19</f>
+        <f t="shared" si="1"/>
         <v>41.751673604727138</v>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
         <v>50000</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>833333333.33333325</v>
       </c>
       <c r="C20" s="2">
@@ -1614,34 +1614,34 @@
         <v>8333333333.3333321</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>264.5502645502645</v>
       </c>
       <c r="J20" s="2">
-        <f xml:space="preserve"> I20/(SQRT(2.65 * 9.81 * (D20^5)))</f>
+        <f t="shared" si="13"/>
         <v>1882879.8677232719</v>
       </c>
       <c r="K20" s="4">
         <v>1.36807554819461E-3</v>
       </c>
       <c r="L20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8848203916580557E-2</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>171.31954532933048</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.62627510407090703</v>
       </c>
       <c r="O20" s="2">
-        <f>M20/D20</f>
+        <f t="shared" si="0"/>
         <v>11421.303021955366</v>
       </c>
       <c r="P20" s="2">
-        <f>N20/D20</f>
+        <f t="shared" si="1"/>
         <v>41.751673604727138</v>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
         <v>100000</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C21" s="2">
@@ -1673,34 +1673,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J21" s="2">
-        <f xml:space="preserve"> I21/(SQRT(2.65 * 9.81 * (D21^5)))</f>
+        <f t="shared" si="13"/>
         <v>7531519.4708930878</v>
       </c>
       <c r="K21" s="4">
         <v>7.5571013181615796E-4</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4870245382867584E-2</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>342.88850750472051</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.97742012019346347</v>
       </c>
       <c r="O21" s="2">
-        <f>M21/D21</f>
+        <f t="shared" si="0"/>
         <v>22859.233833648035</v>
       </c>
       <c r="P21" s="2">
-        <f>N21/D21</f>
+        <f t="shared" si="1"/>
         <v>65.161341346230898</v>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
         <v>100000</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C22" s="2">
@@ -1732,34 +1732,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J22" s="2">
-        <f xml:space="preserve"> I22/(SQRT(2.65 * 9.81 * (D22^5)))</f>
+        <f t="shared" si="13"/>
         <v>20754427.152964957</v>
       </c>
       <c r="K22" s="4">
         <v>7.5571013181615796E-4</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4870245382867584E-2</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>629.92641153828367</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.65161341346230894</v>
       </c>
       <c r="O22" s="2">
-        <f>M22/D22</f>
+        <f t="shared" si="0"/>
         <v>62992.641153828365</v>
       </c>
       <c r="P22" s="2">
-        <f>N22/D22</f>
+        <f t="shared" si="1"/>
         <v>65.161341346230898</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>100000</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C23" s="2">
@@ -1791,34 +1791,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J23" s="2">
-        <f xml:space="preserve"> I23/(SQRT(2.65 * 9.81 * (D23^5)))</f>
+        <f t="shared" si="13"/>
         <v>42604707.924056165</v>
       </c>
       <c r="K23" s="4">
         <v>7.5571013181615796E-4</v>
       </c>
       <c r="L23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4870245382867584E-2</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>969.83515539008829</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.48871006009673174</v>
       </c>
       <c r="O23" s="2">
-        <f>M23/D23</f>
+        <f t="shared" si="0"/>
         <v>129311.35405201178</v>
       </c>
       <c r="P23" s="2">
-        <f>N23/D23</f>
+        <f t="shared" si="1"/>
         <v>65.161341346230898</v>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
         <v>100000</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C24" s="2">
@@ -1850,34 +1850,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J24" s="2">
-        <f xml:space="preserve"> I24/(SQRT(2.65 * 9.81 * (D24^5)))</f>
+        <f t="shared" si="13"/>
         <v>117404769.43602987</v>
       </c>
       <c r="K24" s="4">
         <v>7.5571013181615796E-4</v>
       </c>
       <c r="L24" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4870245382867584E-2</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1781.7009489889113</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.32580670673115447</v>
       </c>
       <c r="O24" s="2">
-        <f>M24/D24</f>
+        <f t="shared" si="0"/>
         <v>356340.18979778222</v>
       </c>
       <c r="P24" s="2">
-        <f>N24/D24</f>
+        <f t="shared" si="1"/>
         <v>65.161341346230898</v>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
         <v>100000</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C25" s="2">
@@ -1909,34 +1909,34 @@
         <v>16666666666.666664</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>529.100529100529</v>
       </c>
       <c r="J25" s="2">
-        <f xml:space="preserve"> I25/(SQRT(2.65 * 9.81 * (D25^5)))</f>
+        <f t="shared" si="13"/>
         <v>3765759.7354465439</v>
       </c>
       <c r="K25" s="4">
         <v>1.3689290994261601E-3</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8852702509712405E-2</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>342.88850750658469</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.62598221112961361</v>
       </c>
       <c r="O25" s="2">
-        <f>M25/D25</f>
+        <f t="shared" si="0"/>
         <v>22859.233833772312</v>
       </c>
       <c r="P25" s="2">
-        <f>N25/D25</f>
+        <f t="shared" si="1"/>
         <v>41.732147408640905</v>
       </c>
     </row>
@@ -1945,7 +1945,7 @@
         <v>100000</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C26" s="2">
@@ -1968,34 +1968,34 @@
         <v>16666666666.666664</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>529.100529100529</v>
       </c>
       <c r="J26" s="2">
-        <f xml:space="preserve"> I26/(SQRT(2.65 * 9.81 * (D26^5)))</f>
+        <f t="shared" si="13"/>
         <v>665698.56131337758</v>
       </c>
       <c r="K26" s="4">
         <v>1.3689290994261601E-3</v>
       </c>
       <c r="L26" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8852702509712405E-2</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>121.22939442442009</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.2519644222592272</v>
       </c>
       <c r="O26" s="2">
-        <f>M26/D26</f>
+        <f t="shared" si="0"/>
         <v>4040.9798141473366</v>
       </c>
       <c r="P26" s="2">
-        <f>N26/D26</f>
+        <f t="shared" si="1"/>
         <v>41.732147408640905</v>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
         <v>100000</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C27" s="2">
@@ -2027,34 +2027,34 @@
         <v>3333333333.333333</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>105.82010582010581</v>
       </c>
       <c r="J27" s="2">
-        <f xml:space="preserve"> I27/(SQRT(2.65 * 9.81 * (D27^5)))</f>
+        <f t="shared" si="13"/>
         <v>133139.71226267552</v>
       </c>
       <c r="K27" s="4">
         <v>5.4387375481128397E-3</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.0734818403028075E-2</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>121.22939442412066</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.44489151972031621</v>
       </c>
       <c r="O27" s="2">
-        <f>M27/D27</f>
+        <f t="shared" si="0"/>
         <v>4040.9798141373553</v>
       </c>
       <c r="P27" s="2">
-        <f>N27/D27</f>
+        <f t="shared" si="1"/>
         <v>14.829717324010542</v>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
         <v>100000</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C28" s="2">
@@ -2086,34 +2086,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J28" s="2">
-        <f xml:space="preserve"> I28/(SQRT(2.65 * 9.81 * (D28^5)))</f>
+        <f t="shared" si="13"/>
         <v>1331397.1226267552</v>
       </c>
       <c r="K28" s="4">
         <v>7.5571013181615796E-4</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.4870245382867584E-2</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>121.22939442376101</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.9548402403869269</v>
       </c>
       <c r="O28" s="2">
-        <f>M28/D28</f>
+        <f t="shared" si="0"/>
         <v>4040.9798141253673</v>
       </c>
       <c r="P28" s="2">
-        <f>N28/D28</f>
+        <f t="shared" si="1"/>
         <v>65.161341346230898</v>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
         <v>100000</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C29" s="2">
@@ -2145,34 +2145,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J29" s="2">
-        <f xml:space="preserve"> I29/(SQRT(2.65 * 9.81 * (D29^5)))</f>
+        <f t="shared" si="13"/>
         <v>1331397.1226267552</v>
       </c>
       <c r="K29" s="4">
         <v>2.6125306266694599E-3</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.3912250115070215E-2</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>515.34544152470266</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.77104843720174043</v>
       </c>
       <c r="O29" s="2">
-        <f>M29/D29</f>
+        <f t="shared" si="0"/>
         <v>17178.181384156756</v>
       </c>
       <c r="P29" s="2">
-        <f>N29/D29</f>
+        <f t="shared" si="1"/>
         <v>25.70161457339135</v>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
         <v>100000</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C30" s="2">
@@ -2204,34 +2204,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J30" s="2">
-        <f xml:space="preserve"> I30/(SQRT(2.65 * 9.81 * (D30^5)))</f>
+        <f t="shared" si="13"/>
         <v>1331397.1226267552</v>
       </c>
       <c r="K30" s="4">
         <v>1.0041315013884699E-2</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.7483082758093514E-2</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2479.0341376275987</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.28088901821431705</v>
       </c>
       <c r="O30" s="2">
-        <f>M30/D30</f>
+        <f t="shared" si="0"/>
         <v>82634.471254253294</v>
       </c>
       <c r="P30" s="2">
-        <f>N30/D30</f>
+        <f t="shared" si="1"/>
         <v>9.3629672738105683</v>
       </c>
     </row>
@@ -2240,7 +2240,7 @@
         <v>100000</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3333333333.333333</v>
       </c>
       <c r="C31" s="2">
@@ -2263,34 +2263,34 @@
         <v>33333333333.333328</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1058.201058201058</v>
       </c>
       <c r="J31" s="2">
-        <f xml:space="preserve"> I31/(SQRT(2.65 * 9.81 * (D31^5)))</f>
+        <f t="shared" si="13"/>
         <v>1331397.1226267552</v>
       </c>
       <c r="K31" s="4">
         <v>2.9170189776050299E-4</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9603159461957901E-2</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>39.929077850756471</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.9918412632211715</v>
       </c>
       <c r="O31" s="2">
-        <f>M31/D31</f>
+        <f t="shared" si="0"/>
         <v>1330.9692616918824</v>
       </c>
       <c r="P31" s="2">
-        <f>N31/D31</f>
+        <f t="shared" si="1"/>
         <v>133.06137544070572</v>
       </c>
     </row>

</xml_diff>